<commit_message>
collect updated death totals
</commit_message>
<xml_diff>
--- a/data/04_deaths/deaths_total_fhi.xlsx
+++ b/data/04_deaths/deaths_total_fhi.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B242"/>
+  <dimension ref="A1:B297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,2412 +446,2962 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-28</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-27</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-26</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-22</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-21</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-20</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-19</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-16</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-15</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-14</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-13</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-09</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-08</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-07</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>2021-04-01</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-30</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-29</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-26</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-25</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-24</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-22</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-19</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-18</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-16</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-15</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-12</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-11</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-10</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-09</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-08</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-05</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-04</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-03</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-02</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>2021-03-01</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-26</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-25</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-24</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-23</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-22</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-19</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-18</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-17</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-16</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-15</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-12</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>2021-02-11</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
         <is>
           <t>2021-02-10</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B57" t="n">
         <v>592</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
         <is>
           <t>2021-02-09</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B58" t="n">
         <v>583</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
         <is>
           <t>2021-02-08</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B59" t="n">
         <v>582</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
         <is>
           <t>2021-02-05</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B60" t="n">
         <v>582</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
         <is>
           <t>2021-02-04</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B61" t="n">
         <v>582</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
         <is>
           <t>2021-02-03</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B62" t="n">
         <v>574</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
         <is>
           <t>2021-02-02</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B63" t="n">
         <v>568</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
         <is>
           <t>2021-02-01</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B64" t="n">
         <v>567</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
         <is>
           <t>2021-01-29</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B65" t="n">
         <v>564</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
         <is>
           <t>2021-01-28</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B66" t="n">
         <v>557</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
         <is>
           <t>2021-01-27</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B67" t="n">
         <v>556</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
         <is>
           <t>2021-01-26</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B68" t="n">
         <v>550</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
         <is>
           <t>2021-01-25</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B69" t="n">
         <v>548</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
         <is>
           <t>2021-01-22</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B70" t="n">
         <v>544</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
         <is>
           <t>2021-01-21</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B71" t="n">
         <v>544</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
         <is>
           <t>2021-01-20</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B72" t="n">
         <v>543</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
         <is>
           <t>2021-01-19</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B73" t="n">
         <v>525</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
         <is>
           <t>2021-01-18</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B74" t="n">
         <v>521</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
         <is>
           <t>2021-01-15</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B75" t="n">
         <v>517</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
         <is>
           <t>2021-01-14</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B76" t="n">
         <v>511</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
         <is>
           <t>2021-01-13</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B77" t="n">
         <v>508</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
         <is>
           <t>2021-01-12</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B78" t="n">
         <v>482</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
         <is>
           <t>2021-01-11</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B79" t="n">
         <v>478</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
         <is>
           <t>2021-01-08</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B80" t="n">
         <v>472</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
         <is>
           <t>2021-01-07</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B81" t="n">
         <v>467</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
         <is>
           <t>2021-01-06</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B82" t="n">
         <v>466</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
         <is>
           <t>2021-01-05</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B83" t="n">
         <v>452</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
         <is>
           <t>2021-01-04</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B84" t="n">
         <v>449</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
         <is>
           <t>2020-12-30</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B85" t="n">
         <v>436</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
         <is>
           <t>2020-12-29</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B86" t="n">
         <v>433</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
         <is>
           <t>2020-12-28</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B87" t="n">
         <v>429</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
         <is>
           <t>2020-12-23</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B88" t="n">
         <v>421</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
         <is>
           <t>2020-12-22</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B89" t="n">
         <v>405</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
         <is>
           <t>2020-12-21</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B90" t="n">
         <v>405</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
         <is>
           <t>2020-12-18</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B91" t="n">
         <v>404</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
         <is>
           <t>2020-12-17</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B92" t="n">
         <v>404</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
         <is>
           <t>2020-12-16</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B93" t="n">
         <v>402</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
         <is>
           <t>2020-12-15</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B94" t="n">
         <v>395</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
         <is>
           <t>2020-12-14</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B95" t="n">
         <v>393</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
         <is>
           <t>2020-12-11</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B96" t="n">
         <v>387</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
         <is>
           <t>2020-12-10</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B97" t="n">
         <v>382</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
         <is>
           <t>2020-12-09</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B98" t="n">
         <v>361</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
         <is>
           <t>2020-12-08</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B99" t="n">
         <v>361</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
         <is>
           <t>2020-12-07</t>
         </is>
       </c>
-      <c r="B45" t="n">
+      <c r="B100" t="n">
         <v>359</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
         <is>
           <t>2020-12-04</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="B101" t="n">
         <v>354</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
         <is>
           <t>2020-12-03</t>
         </is>
       </c>
-      <c r="B47" t="n">
+      <c r="B102" t="n">
         <v>353</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
         <is>
           <t>2020-12-02</t>
         </is>
       </c>
-      <c r="B48" t="n">
+      <c r="B103" t="n">
         <v>351</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
         <is>
           <t>2020-12-01</t>
         </is>
       </c>
-      <c r="B49" t="n">
+      <c r="B104" t="n">
         <v>334</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
         <is>
           <t>2020-11-30</t>
         </is>
       </c>
-      <c r="B50" t="n">
+      <c r="B105" t="n">
         <v>332</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
         <is>
           <t>2020-11-27</t>
         </is>
       </c>
-      <c r="B51" t="n">
+      <c r="B106" t="n">
         <v>328</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
         <is>
           <t>2020-11-26</t>
         </is>
       </c>
-      <c r="B52" t="n">
+      <c r="B107" t="n">
         <v>316</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
         <is>
           <t>2020-11-25</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="B108" t="n">
         <v>316</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
         <is>
           <t>2020-11-24</t>
         </is>
       </c>
-      <c r="B54" t="n">
+      <c r="B109" t="n">
         <v>314</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
         <is>
           <t>2020-11-23</t>
         </is>
       </c>
-      <c r="B55" t="n">
+      <c r="B110" t="n">
         <v>311</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
         <is>
           <t>2020-11-20</t>
         </is>
       </c>
-      <c r="B56" t="n">
+      <c r="B111" t="n">
         <v>306</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
         <is>
           <t>2020-11-19</t>
         </is>
       </c>
-      <c r="B57" t="n">
+      <c r="B112" t="n">
         <v>305</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
         <is>
           <t>2020-11-18</t>
         </is>
       </c>
-      <c r="B58" t="n">
+      <c r="B113" t="n">
         <v>299</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
         <is>
           <t>2020-11-17</t>
         </is>
       </c>
-      <c r="B59" t="n">
+      <c r="B114" t="n">
         <v>298</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
         <is>
           <t>2020-11-16</t>
         </is>
       </c>
-      <c r="B60" t="n">
+      <c r="B115" t="n">
         <v>294</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
         <is>
           <t>2020-11-13</t>
         </is>
       </c>
-      <c r="B61" t="n">
+      <c r="B116" t="n">
         <v>294</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
         <is>
           <t>2020-11-12</t>
         </is>
       </c>
-      <c r="B62" t="n">
+      <c r="B117" t="n">
         <v>291</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
         <is>
           <t>2020-11-11</t>
         </is>
       </c>
-      <c r="B63" t="n">
+      <c r="B118" t="n">
         <v>285</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
         <is>
           <t>2020-11-10</t>
         </is>
       </c>
-      <c r="B64" t="n">
+      <c r="B119" t="n">
         <v>285</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
         <is>
           <t>2020-11-09</t>
         </is>
       </c>
-      <c r="B65" t="n">
+      <c r="B120" t="n">
         <v>285</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
         <is>
           <t>2020-11-06</t>
         </is>
       </c>
-      <c r="B66" t="n">
+      <c r="B121" t="n">
         <v>285</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
         <is>
           <t>2020-11-05</t>
         </is>
       </c>
-      <c r="B67" t="n">
+      <c r="B122" t="n">
         <v>284</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
         <is>
           <t>2020-11-04</t>
         </is>
       </c>
-      <c r="B68" t="n">
+      <c r="B123" t="n">
         <v>282</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
         <is>
           <t>2020-11-03</t>
         </is>
       </c>
-      <c r="B69" t="n">
+      <c r="B124" t="n">
         <v>282</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
         <is>
           <t>2020-11-02</t>
         </is>
       </c>
-      <c r="B70" t="n">
+      <c r="B125" t="n">
         <v>282</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
         <is>
           <t>2020-10-30</t>
         </is>
       </c>
-      <c r="B71" t="n">
+      <c r="B126" t="n">
         <v>282</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
         <is>
           <t>2020-10-29</t>
         </is>
       </c>
-      <c r="B72" t="n">
+      <c r="B127" t="n">
         <v>281</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
         <is>
           <t>2020-10-28</t>
         </is>
       </c>
-      <c r="B73" t="n">
+      <c r="B128" t="n">
         <v>280</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
         <is>
           <t>2020-10-27</t>
         </is>
       </c>
-      <c r="B74" t="n">
+      <c r="B129" t="n">
         <v>280</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
         <is>
           <t>2020-10-26</t>
         </is>
       </c>
-      <c r="B75" t="n">
+      <c r="B130" t="n">
         <v>279</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
         <is>
           <t>2020-10-23</t>
         </is>
       </c>
-      <c r="B76" t="n">
+      <c r="B131" t="n">
         <v>279</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
         <is>
           <t>2020-10-22</t>
         </is>
       </c>
-      <c r="B77" t="n">
+      <c r="B132" t="n">
         <v>279</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
         <is>
           <t>2020-10-21</t>
         </is>
       </c>
-      <c r="B78" t="n">
+      <c r="B133" t="n">
         <v>279</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
         <is>
           <t>2020-10-20</t>
         </is>
       </c>
-      <c r="B79" t="n">
+      <c r="B134" t="n">
         <v>278</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr">
         <is>
           <t>2020-10-19</t>
         </is>
       </c>
-      <c r="B80" t="n">
+      <c r="B135" t="n">
         <v>278</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
         <is>
           <t>2020-10-16</t>
         </is>
       </c>
-      <c r="B81" t="n">
+      <c r="B136" t="n">
         <v>278</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr">
         <is>
           <t>2020-10-15</t>
         </is>
       </c>
-      <c r="B82" t="n">
+      <c r="B137" t="n">
         <v>278</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr">
         <is>
           <t>2020-10-14</t>
         </is>
       </c>
-      <c r="B83" t="n">
+      <c r="B138" t="n">
         <v>277</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr">
         <is>
           <t>2020-10-13</t>
         </is>
       </c>
-      <c r="B84" t="n">
+      <c r="B139" t="n">
         <v>277</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr">
         <is>
           <t>2020-10-12</t>
         </is>
       </c>
-      <c r="B85" t="n">
+      <c r="B140" t="n">
         <v>276</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
         <is>
           <t>2020-10-09</t>
         </is>
       </c>
-      <c r="B86" t="n">
+      <c r="B141" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr">
         <is>
           <t>2020-10-08</t>
         </is>
       </c>
-      <c r="B87" t="n">
+      <c r="B142" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr">
         <is>
           <t>2020-10-07</t>
         </is>
       </c>
-      <c r="B88" t="n">
+      <c r="B143" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr">
         <is>
           <t>2020-10-06</t>
         </is>
       </c>
-      <c r="B89" t="n">
+      <c r="B144" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
         <is>
           <t>2020-10-05</t>
         </is>
       </c>
-      <c r="B90" t="n">
+      <c r="B145" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
         <is>
           <t>2020-10-02</t>
         </is>
       </c>
-      <c r="B91" t="n">
+      <c r="B146" t="n">
         <v>275</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
         <is>
           <t>2020-10-01</t>
         </is>
       </c>
-      <c r="B92" t="n">
+      <c r="B147" t="n">
         <v>274</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
         <is>
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="B93" t="n">
+      <c r="B148" t="n">
         <v>274</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
         <is>
           <t>2020-09-29</t>
         </is>
       </c>
-      <c r="B94" t="n">
+      <c r="B149" t="n">
         <v>274</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
         <is>
           <t>2020-09-28</t>
         </is>
       </c>
-      <c r="B95" t="n">
+      <c r="B150" t="n">
         <v>274</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
+    <row r="151">
+      <c r="A151" s="1" t="inlineStr">
         <is>
           <t>2020-09-25</t>
         </is>
       </c>
-      <c r="B96" t="n">
+      <c r="B151" t="n">
         <v>270</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
         <is>
           <t>2020-09-24</t>
         </is>
       </c>
-      <c r="B97" t="n">
+      <c r="B152" t="n">
         <v>270</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
         <is>
           <t>2020-09-23</t>
         </is>
       </c>
-      <c r="B98" t="n">
+      <c r="B153" t="n">
         <v>267</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
         <is>
           <t>2020-09-22</t>
         </is>
       </c>
-      <c r="B99" t="n">
+      <c r="B154" t="n">
         <v>267</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
         <is>
           <t>2020-09-21</t>
         </is>
       </c>
-      <c r="B100" t="n">
+      <c r="B155" t="n">
         <v>267</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
+    <row r="156">
+      <c r="A156" s="1" t="inlineStr">
         <is>
           <t>2020-09-18</t>
         </is>
       </c>
-      <c r="B101" t="n">
+      <c r="B156" t="n">
         <v>267</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
+    <row r="157">
+      <c r="A157" s="1" t="inlineStr">
         <is>
           <t>2020-09-17</t>
         </is>
       </c>
-      <c r="B102" t="n">
+      <c r="B157" t="n">
         <v>266</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
+    <row r="158">
+      <c r="A158" s="1" t="inlineStr">
         <is>
           <t>2020-09-16</t>
         </is>
       </c>
-      <c r="B103" t="n">
+      <c r="B158" t="n">
         <v>265</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
+    <row r="159">
+      <c r="A159" s="1" t="inlineStr">
         <is>
           <t>2020-09-15</t>
         </is>
       </c>
-      <c r="B104" t="n">
+      <c r="B159" t="n">
         <v>265</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
         <is>
           <t>2020-09-14</t>
         </is>
       </c>
-      <c r="B105" t="n">
+      <c r="B160" t="n">
         <v>265</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
         <is>
           <t>2020-09-11</t>
         </is>
       </c>
-      <c r="B106" t="n">
+      <c r="B161" t="n">
         <v>265</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
         <is>
           <t>2020-09-10</t>
         </is>
       </c>
-      <c r="B107" t="n">
+      <c r="B162" t="n">
         <v>265</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
         <is>
           <t>2020-09-09</t>
         </is>
       </c>
-      <c r="B108" t="n">
+      <c r="B163" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
         <is>
           <t>2020-09-08</t>
         </is>
       </c>
-      <c r="B109" t="n">
+      <c r="B164" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
         <is>
           <t>2020-09-07</t>
         </is>
       </c>
-      <c r="B110" t="n">
+      <c r="B165" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
         <is>
           <t>2020-09-04</t>
         </is>
       </c>
-      <c r="B111" t="n">
+      <c r="B166" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
         <is>
           <t>2020-09-03</t>
         </is>
       </c>
-      <c r="B112" t="n">
+      <c r="B167" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
         <is>
           <t>2020-09-02</t>
         </is>
       </c>
-      <c r="B113" t="n">
+      <c r="B168" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
+    <row r="169">
+      <c r="A169" s="1" t="inlineStr">
         <is>
           <t>2020-09-01</t>
         </is>
       </c>
-      <c r="B114" t="n">
+      <c r="B169" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
+    <row r="170">
+      <c r="A170" s="1" t="inlineStr">
         <is>
           <t>2020-08-31</t>
         </is>
       </c>
-      <c r="B115" t="n">
+      <c r="B170" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
+    <row r="171">
+      <c r="A171" s="1" t="inlineStr">
         <is>
           <t>2020-08-28</t>
         </is>
       </c>
-      <c r="B116" t="n">
+      <c r="B171" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
+    <row r="172">
+      <c r="A172" s="1" t="inlineStr">
         <is>
           <t>2020-08-27</t>
         </is>
       </c>
-      <c r="B117" t="n">
+      <c r="B172" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
+    <row r="173">
+      <c r="A173" s="1" t="inlineStr">
         <is>
           <t>2020-08-26</t>
         </is>
       </c>
-      <c r="B118" t="n">
+      <c r="B173" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
+    <row r="174">
+      <c r="A174" s="1" t="inlineStr">
         <is>
           <t>2020-08-25</t>
         </is>
       </c>
-      <c r="B119" t="n">
+      <c r="B174" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
         <is>
           <t>2020-08-24</t>
         </is>
       </c>
-      <c r="B120" t="n">
+      <c r="B175" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
         <is>
           <t>2020-08-21</t>
         </is>
       </c>
-      <c r="B121" t="n">
+      <c r="B176" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
         <is>
           <t>2020-08-20</t>
         </is>
       </c>
-      <c r="B122" t="n">
+      <c r="B177" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
         <is>
           <t>2020-08-19</t>
         </is>
       </c>
-      <c r="B123" t="n">
+      <c r="B178" t="n">
         <v>262</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
         <is>
           <t>2020-08-18</t>
         </is>
       </c>
-      <c r="B124" t="n">
+      <c r="B179" t="n">
         <v>262</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
         <is>
           <t>2020-08-17</t>
         </is>
       </c>
-      <c r="B125" t="n">
+      <c r="B180" t="n">
         <v>261</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
+    <row r="181">
+      <c r="A181" s="1" t="inlineStr">
         <is>
           <t>2020-08-14</t>
         </is>
       </c>
-      <c r="B126" t="n">
+      <c r="B181" t="n">
         <v>261</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
+    <row r="182">
+      <c r="A182" s="1" t="inlineStr">
         <is>
           <t>2020-08-13</t>
         </is>
       </c>
-      <c r="B127" t="n">
+      <c r="B182" t="n">
         <v>257</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
+    <row r="183">
+      <c r="A183" s="1" t="inlineStr">
         <is>
           <t>2020-08-12</t>
         </is>
       </c>
-      <c r="B128" t="n">
+      <c r="B183" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
+    <row r="184">
+      <c r="A184" s="1" t="inlineStr">
         <is>
           <t>2020-08-11</t>
         </is>
       </c>
-      <c r="B129" t="n">
+      <c r="B184" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
+    <row r="185">
+      <c r="A185" s="1" t="inlineStr">
         <is>
           <t>2020-08-10</t>
         </is>
       </c>
-      <c r="B130" t="n">
+      <c r="B185" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
+    <row r="186">
+      <c r="A186" s="1" t="inlineStr">
         <is>
           <t>2020-08-07</t>
         </is>
       </c>
-      <c r="B131" t="n">
+      <c r="B186" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
         <is>
           <t>2020-08-06</t>
         </is>
       </c>
-      <c r="B132" t="n">
+      <c r="B187" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
+    <row r="188">
+      <c r="A188" s="1" t="inlineStr">
         <is>
           <t>2020-08-05</t>
         </is>
       </c>
-      <c r="B133" t="n">
+      <c r="B188" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
+    <row r="189">
+      <c r="A189" s="1" t="inlineStr">
         <is>
           <t>2020-08-04</t>
         </is>
       </c>
-      <c r="B134" t="n">
+      <c r="B189" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
         <is>
           <t>2020-08-03</t>
         </is>
       </c>
-      <c r="B135" t="n">
+      <c r="B190" t="n">
         <v>256</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
         <is>
           <t>2020-07-31</t>
         </is>
       </c>
-      <c r="B136" t="n">
+      <c r="B191" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
         <is>
           <t>2020-07-30</t>
         </is>
       </c>
-      <c r="B137" t="n">
+      <c r="B192" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
         <is>
           <t>2020-07-29</t>
         </is>
       </c>
-      <c r="B138" t="n">
+      <c r="B193" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
         <is>
           <t>2020-07-28</t>
         </is>
       </c>
-      <c r="B139" t="n">
+      <c r="B194" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
         <is>
           <t>2020-07-27</t>
         </is>
       </c>
-      <c r="B140" t="n">
+      <c r="B195" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
         <is>
           <t>2020-07-24</t>
         </is>
       </c>
-      <c r="B141" t="n">
+      <c r="B196" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
         <is>
           <t>2020-07-23</t>
         </is>
       </c>
-      <c r="B142" t="n">
+      <c r="B197" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
         <is>
           <t>2020-07-22</t>
         </is>
       </c>
-      <c r="B143" t="n">
+      <c r="B198" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
         <is>
           <t>2020-07-21</t>
         </is>
       </c>
-      <c r="B144" t="n">
+      <c r="B199" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
+    <row r="200">
+      <c r="A200" s="1" t="inlineStr">
         <is>
           <t>2020-07-20</t>
         </is>
       </c>
-      <c r="B145" t="n">
+      <c r="B200" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
+    <row r="201">
+      <c r="A201" s="1" t="inlineStr">
         <is>
           <t>2020-07-17</t>
         </is>
       </c>
-      <c r="B146" t="n">
+      <c r="B201" t="n">
         <v>255</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
+    <row r="202">
+      <c r="A202" s="1" t="inlineStr">
         <is>
           <t>2020-07-16</t>
         </is>
       </c>
-      <c r="B147" t="n">
+      <c r="B202" t="n">
         <v>254</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
+    <row r="203">
+      <c r="A203" s="1" t="inlineStr">
         <is>
           <t>2020-07-15</t>
         </is>
       </c>
-      <c r="B148" t="n">
+      <c r="B203" t="n">
         <v>253</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
+    <row r="204">
+      <c r="A204" s="1" t="inlineStr">
         <is>
           <t>2020-07-14</t>
         </is>
       </c>
-      <c r="B149" t="n">
+      <c r="B204" t="n">
         <v>253</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
+    <row r="205">
+      <c r="A205" s="1" t="inlineStr">
         <is>
           <t>2020-07-13</t>
         </is>
       </c>
-      <c r="B150" t="n">
+      <c r="B205" t="n">
         <v>253</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
+    <row r="206">
+      <c r="A206" s="1" t="inlineStr">
         <is>
           <t>2020-07-10</t>
         </is>
       </c>
-      <c r="B151" t="n">
+      <c r="B206" t="n">
         <v>252</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
+    <row r="207">
+      <c r="A207" s="1" t="inlineStr">
         <is>
           <t>2020-07-09</t>
         </is>
       </c>
-      <c r="B152" t="n">
+      <c r="B207" t="n">
         <v>252</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
+    <row r="208">
+      <c r="A208" s="1" t="inlineStr">
         <is>
           <t>2020-07-08</t>
         </is>
       </c>
-      <c r="B153" t="n">
+      <c r="B208" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
+    <row r="209">
+      <c r="A209" s="1" t="inlineStr">
         <is>
           <t>2020-07-07</t>
         </is>
       </c>
-      <c r="B154" t="n">
+      <c r="B209" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
+    <row r="210">
+      <c r="A210" s="1" t="inlineStr">
         <is>
           <t>2020-07-06</t>
         </is>
       </c>
-      <c r="B155" t="n">
+      <c r="B210" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
+    <row r="211">
+      <c r="A211" s="1" t="inlineStr">
         <is>
           <t>2020-07-03</t>
         </is>
       </c>
-      <c r="B156" t="n">
+      <c r="B211" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
+    <row r="212">
+      <c r="A212" s="1" t="inlineStr">
         <is>
           <t>2020-07-02</t>
         </is>
       </c>
-      <c r="B157" t="n">
+      <c r="B212" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
+    <row r="213">
+      <c r="A213" s="1" t="inlineStr">
         <is>
           <t>2020-07-01</t>
         </is>
       </c>
-      <c r="B158" t="n">
+      <c r="B213" t="n">
         <v>251</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
+    <row r="214">
+      <c r="A214" s="1" t="inlineStr">
         <is>
           <t>2020-06-30</t>
         </is>
       </c>
-      <c r="B159" t="n">
+      <c r="B214" t="n">
         <v>250</v>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
+    <row r="215">
+      <c r="A215" s="1" t="inlineStr">
         <is>
           <t>2020-06-29</t>
         </is>
       </c>
-      <c r="B160" t="n">
+      <c r="B215" t="n">
         <v>249</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
+    <row r="216">
+      <c r="A216" s="1" t="inlineStr">
         <is>
           <t>2020-06-26</t>
         </is>
       </c>
-      <c r="B161" t="n">
+      <c r="B216" t="n">
         <v>249</v>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
+    <row r="217">
+      <c r="A217" s="1" t="inlineStr">
         <is>
           <t>2020-06-25</t>
         </is>
       </c>
-      <c r="B162" t="n">
+      <c r="B217" t="n">
         <v>249</v>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
+    <row r="218">
+      <c r="A218" s="1" t="inlineStr">
         <is>
           <t>2020-06-24</t>
         </is>
       </c>
-      <c r="B163" t="n">
+      <c r="B218" t="n">
         <v>249</v>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
+    <row r="219">
+      <c r="A219" s="1" t="inlineStr">
         <is>
           <t>2020-06-23</t>
         </is>
       </c>
-      <c r="B164" t="n">
+      <c r="B219" t="n">
         <v>248</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
+    <row r="220">
+      <c r="A220" s="1" t="inlineStr">
         <is>
           <t>2020-06-19</t>
         </is>
       </c>
-      <c r="B165" t="n">
+      <c r="B220" t="n">
         <v>244</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
+    <row r="221">
+      <c r="A221" s="1" t="inlineStr">
         <is>
           <t>2020-06-18</t>
         </is>
       </c>
-      <c r="B166" t="n">
+      <c r="B221" t="n">
         <v>244</v>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
+    <row r="222">
+      <c r="A222" s="1" t="inlineStr">
         <is>
           <t>2020-06-16</t>
         </is>
       </c>
-      <c r="B167" t="n">
+      <c r="B222" t="n">
         <v>242</v>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
+    <row r="223">
+      <c r="A223" s="1" t="inlineStr">
         <is>
           <t>2020-06-15</t>
         </is>
       </c>
-      <c r="B168" t="n">
+      <c r="B223" t="n">
         <v>242</v>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
+    <row r="224">
+      <c r="A224" s="1" t="inlineStr">
         <is>
           <t>2020-06-12</t>
         </is>
       </c>
-      <c r="B169" t="n">
+      <c r="B224" t="n">
         <v>242</v>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
+    <row r="225">
+      <c r="A225" s="1" t="inlineStr">
         <is>
           <t>2020-06-11</t>
         </is>
       </c>
-      <c r="B170" t="n">
+      <c r="B225" t="n">
         <v>242</v>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
+    <row r="226">
+      <c r="A226" s="1" t="inlineStr">
         <is>
           <t>2020-06-10</t>
         </is>
       </c>
-      <c r="B171" t="n">
+      <c r="B226" t="n">
         <v>239</v>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
+    <row r="227">
+      <c r="A227" s="1" t="inlineStr">
         <is>
           <t>2020-06-09</t>
         </is>
       </c>
-      <c r="B172" t="n">
+      <c r="B227" t="n">
         <v>239</v>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
+    <row r="228">
+      <c r="A228" s="1" t="inlineStr">
         <is>
           <t>2020-06-08</t>
         </is>
       </c>
-      <c r="B173" t="n">
+      <c r="B228" t="n">
         <v>239</v>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
+    <row r="229">
+      <c r="A229" s="1" t="inlineStr">
         <is>
           <t>2020-06-05</t>
         </is>
       </c>
-      <c r="B174" t="n">
+      <c r="B229" t="n">
         <v>238</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
+    <row r="230">
+      <c r="A230" s="1" t="inlineStr">
         <is>
           <t>2020-06-04</t>
         </is>
       </c>
-      <c r="B175" t="n">
+      <c r="B230" t="n">
         <v>238</v>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
+    <row r="231">
+      <c r="A231" s="1" t="inlineStr">
         <is>
           <t>2020-06-03</t>
         </is>
       </c>
-      <c r="B176" t="n">
+      <c r="B231" t="n">
         <v>237</v>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
+    <row r="232">
+      <c r="A232" s="1" t="inlineStr">
         <is>
           <t>2020-06-02</t>
         </is>
       </c>
-      <c r="B177" t="n">
+      <c r="B232" t="n">
         <v>237</v>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
+    <row r="233">
+      <c r="A233" s="1" t="inlineStr">
         <is>
           <t>2020-05-29</t>
         </is>
       </c>
-      <c r="B178" t="n">
+      <c r="B233" t="n">
         <v>236</v>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
+    <row r="234">
+      <c r="A234" s="1" t="inlineStr">
         <is>
           <t>2020-05-28</t>
         </is>
       </c>
-      <c r="B179" t="n">
+      <c r="B234" t="n">
         <v>236</v>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
+    <row r="235">
+      <c r="A235" s="1" t="inlineStr">
         <is>
           <t>2020-05-27</t>
         </is>
       </c>
-      <c r="B180" t="n">
+      <c r="B235" t="n">
         <v>235</v>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
+    <row r="236">
+      <c r="A236" s="1" t="inlineStr">
         <is>
           <t>2020-05-26</t>
         </is>
       </c>
-      <c r="B181" t="n">
+      <c r="B236" t="n">
         <v>235</v>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
+    <row r="237">
+      <c r="A237" s="1" t="inlineStr">
         <is>
           <t>2020-05-25</t>
         </is>
       </c>
-      <c r="B182" t="n">
+      <c r="B237" t="n">
         <v>235</v>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
+    <row r="238">
+      <c r="A238" s="1" t="inlineStr">
         <is>
           <t>2020-05-22</t>
         </is>
       </c>
-      <c r="B183" t="n">
+      <c r="B238" t="n">
         <v>235</v>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
+    <row r="239">
+      <c r="A239" s="1" t="inlineStr">
         <is>
           <t>2020-05-20</t>
         </is>
       </c>
-      <c r="B184" t="n">
+      <c r="B239" t="n">
         <v>234</v>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
+    <row r="240">
+      <c r="A240" s="1" t="inlineStr">
         <is>
           <t>2020-05-19</t>
         </is>
       </c>
-      <c r="B185" t="n">
+      <c r="B240" t="n">
         <v>233</v>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
+    <row r="241">
+      <c r="A241" s="1" t="inlineStr">
         <is>
           <t>2020-05-18</t>
         </is>
       </c>
-      <c r="B186" t="n">
+      <c r="B241" t="n">
         <v>233</v>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
+    <row r="242">
+      <c r="A242" s="1" t="inlineStr">
         <is>
           <t>2020-05-15</t>
         </is>
       </c>
-      <c r="B187" t="n">
+      <c r="B242" t="n">
         <v>232</v>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
+    <row r="243">
+      <c r="A243" s="1" t="inlineStr">
         <is>
           <t>2020-05-14</t>
         </is>
       </c>
-      <c r="B188" t="n">
+      <c r="B243" t="n">
         <v>232</v>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
+    <row r="244">
+      <c r="A244" s="1" t="inlineStr">
         <is>
           <t>2020-05-13</t>
         </is>
       </c>
-      <c r="B189" t="n">
+      <c r="B244" t="n">
         <v>229</v>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
+    <row r="245">
+      <c r="A245" s="1" t="inlineStr">
         <is>
           <t>2020-05-12</t>
         </is>
       </c>
-      <c r="B190" t="n">
+      <c r="B245" t="n">
         <v>228</v>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
+    <row r="246">
+      <c r="A246" s="1" t="inlineStr">
         <is>
           <t>2020-05-11</t>
         </is>
       </c>
-      <c r="B191" t="n">
+      <c r="B246" t="n">
         <v>224</v>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
+    <row r="247">
+      <c r="A247" s="1" t="inlineStr">
         <is>
           <t>2020-05-08</t>
         </is>
       </c>
-      <c r="B192" t="n">
+      <c r="B247" t="n">
         <v>213</v>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
+    <row r="248">
+      <c r="A248" s="1" t="inlineStr">
         <is>
           <t>2020-05-07</t>
         </is>
       </c>
-      <c r="B193" t="n">
+      <c r="B248" t="n">
         <v>209</v>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
+    <row r="249">
+      <c r="A249" s="1" t="inlineStr">
         <is>
           <t>2020-05-06</t>
         </is>
       </c>
-      <c r="B194" t="n">
+      <c r="B249" t="n">
         <v>209</v>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
+    <row r="250">
+      <c r="A250" s="1" t="inlineStr">
         <is>
           <t>2020-05-05</t>
         </is>
       </c>
-      <c r="B195" t="n">
+      <c r="B250" t="n">
         <v>209</v>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
+    <row r="251">
+      <c r="A251" s="1" t="inlineStr">
         <is>
           <t>2020-05-04</t>
         </is>
       </c>
-      <c r="B196" t="n">
+      <c r="B251" t="n">
         <v>208</v>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
+    <row r="252">
+      <c r="A252" s="1" t="inlineStr">
         <is>
           <t>2020-04-30</t>
         </is>
       </c>
-      <c r="B197" t="n">
+      <c r="B252" t="n">
         <v>204</v>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
+    <row r="253">
+      <c r="A253" s="1" t="inlineStr">
         <is>
           <t>2020-04-29</t>
         </is>
       </c>
-      <c r="B198" t="n">
+      <c r="B253" t="n">
         <v>202</v>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
+    <row r="254">
+      <c r="A254" s="1" t="inlineStr">
         <is>
           <t>2020-04-28</t>
         </is>
       </c>
-      <c r="B199" t="n">
+      <c r="B254" t="n">
         <v>195</v>
       </c>
     </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
+    <row r="255">
+      <c r="A255" s="1" t="inlineStr">
         <is>
           <t>2020-04-27</t>
         </is>
       </c>
-      <c r="B200" t="n">
+      <c r="B255" t="n">
         <v>193</v>
       </c>
     </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
+    <row r="256">
+      <c r="A256" s="1" t="inlineStr">
         <is>
           <t>2020-04-24</t>
         </is>
       </c>
-      <c r="B201" t="n">
+      <c r="B256" t="n">
         <v>191</v>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
+    <row r="257">
+      <c r="A257" s="1" t="inlineStr">
         <is>
           <t>2020-04-23</t>
         </is>
       </c>
-      <c r="B202" t="n">
+      <c r="B257" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
+    <row r="258">
+      <c r="A258" s="1" t="inlineStr">
         <is>
           <t>2020-04-22</t>
         </is>
       </c>
-      <c r="B203" t="n">
+      <c r="B258" t="n">
         <v>169</v>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
+    <row r="259">
+      <c r="A259" s="1" t="inlineStr">
         <is>
           <t>2020-04-21</t>
         </is>
       </c>
-      <c r="B204" t="n">
+      <c r="B259" t="n">
         <v>163</v>
       </c>
     </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
+    <row r="260">
+      <c r="A260" s="1" t="inlineStr">
         <is>
           <t>2020-04-20</t>
         </is>
       </c>
-      <c r="B205" t="n">
+      <c r="B260" t="n">
         <v>154</v>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
+    <row r="261">
+      <c r="A261" s="1" t="inlineStr">
         <is>
           <t>2020-04-19</t>
         </is>
       </c>
-      <c r="B206" t="n">
+      <c r="B261" t="n">
         <v>154</v>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
+    <row r="262">
+      <c r="A262" s="1" t="inlineStr">
         <is>
           <t>2020-04-18</t>
         </is>
       </c>
-      <c r="B207" t="n">
+      <c r="B262" t="n">
         <v>148</v>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
+    <row r="263">
+      <c r="A263" s="1" t="inlineStr">
         <is>
           <t>2020-04-17</t>
         </is>
       </c>
-      <c r="B208" t="n">
+      <c r="B263" t="n">
         <v>137</v>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
+    <row r="264">
+      <c r="A264" s="1" t="inlineStr">
         <is>
           <t>2020-04-16</t>
         </is>
       </c>
-      <c r="B209" t="n">
+      <c r="B264" t="n">
         <v>136</v>
       </c>
     </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
+    <row r="265">
+      <c r="A265" s="1" t="inlineStr">
         <is>
           <t>2020-04-15</t>
         </is>
       </c>
-      <c r="B210" t="n">
+      <c r="B265" t="n">
         <v>130</v>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
+    <row r="266">
+      <c r="A266" s="1" t="inlineStr">
         <is>
           <t>2020-04-14</t>
         </is>
       </c>
-      <c r="B211" t="n">
+      <c r="B266" t="n">
         <v>127</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
+    <row r="267">
+      <c r="A267" s="1" t="inlineStr">
         <is>
           <t>2020-04-13</t>
         </is>
       </c>
-      <c r="B212" t="n">
+      <c r="B267" t="n">
         <v>114</v>
       </c>
     </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
+    <row r="268">
+      <c r="A268" s="1" t="inlineStr">
         <is>
           <t>2020-04-12</t>
         </is>
       </c>
-      <c r="B213" t="n">
+      <c r="B268" t="n">
         <v>103</v>
       </c>
     </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
+    <row r="269">
+      <c r="A269" s="1" t="inlineStr">
         <is>
           <t>2020-04-11</t>
         </is>
       </c>
-      <c r="B214" t="n">
+      <c r="B269" t="n">
         <v>98</v>
       </c>
     </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
+    <row r="270">
+      <c r="A270" s="1" t="inlineStr">
         <is>
           <t>2020-04-09</t>
         </is>
       </c>
-      <c r="B215" t="n">
+      <c r="B270" t="n">
         <v>88</v>
       </c>
     </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
+    <row r="271">
+      <c r="A271" s="1" t="inlineStr">
         <is>
           <t>2020-04-07</t>
         </is>
       </c>
-      <c r="B216" t="n">
+      <c r="B271" t="n">
         <v>69</v>
       </c>
     </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
+    <row r="272">
+      <c r="A272" s="1" t="inlineStr">
         <is>
           <t>2020-04-05</t>
         </is>
       </c>
-      <c r="B217" t="n">
+      <c r="B272" t="n">
         <v>58</v>
       </c>
     </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
+    <row r="273">
+      <c r="A273" s="1" t="inlineStr">
         <is>
           <t>2020-04-04</t>
         </is>
       </c>
-      <c r="B218" t="n">
+      <c r="B273" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
+    <row r="274">
+      <c r="A274" s="1" t="inlineStr">
         <is>
           <t>2020-04-02</t>
         </is>
       </c>
-      <c r="B219" t="n">
+      <c r="B274" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
+    <row r="275">
+      <c r="A275" s="1" t="inlineStr">
         <is>
           <t>2020-04-01</t>
         </is>
       </c>
-      <c r="B220" t="n">
+      <c r="B275" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
+    <row r="276">
+      <c r="A276" s="1" t="inlineStr">
         <is>
           <t>2020-03-31</t>
         </is>
       </c>
-      <c r="B221" t="n">
+      <c r="B276" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
+    <row r="277">
+      <c r="A277" s="1" t="inlineStr">
         <is>
           <t>2020-03-30</t>
         </is>
       </c>
-      <c r="B222" t="n">
+      <c r="B277" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
+    <row r="278">
+      <c r="A278" s="1" t="inlineStr">
         <is>
           <t>2020-03-29</t>
         </is>
       </c>
-      <c r="B223" t="n">
+      <c r="B278" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
+    <row r="279">
+      <c r="A279" s="1" t="inlineStr">
         <is>
           <t>2020-03-28</t>
         </is>
       </c>
-      <c r="B224" t="n">
+      <c r="B279" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
+    <row r="280">
+      <c r="A280" s="1" t="inlineStr">
         <is>
           <t>2020-03-27</t>
         </is>
       </c>
-      <c r="B225" t="n">
+      <c r="B280" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
+    <row r="281">
+      <c r="A281" s="1" t="inlineStr">
         <is>
           <t>2020-03-26</t>
         </is>
       </c>
-      <c r="B226" t="n">
+      <c r="B281" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
+    <row r="282">
+      <c r="A282" s="1" t="inlineStr">
         <is>
           <t>2020-03-25</t>
         </is>
       </c>
-      <c r="B227" t="n">
+      <c r="B282" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
+    <row r="283">
+      <c r="A283" s="1" t="inlineStr">
         <is>
           <t>2020-03-24</t>
         </is>
       </c>
-      <c r="B228" t="n">
+      <c r="B283" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
+    <row r="284">
+      <c r="A284" s="1" t="inlineStr">
         <is>
           <t>2020-03-23</t>
         </is>
       </c>
-      <c r="B229" t="n">
+      <c r="B284" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
+    <row r="285">
+      <c r="A285" s="1" t="inlineStr">
         <is>
           <t>2020-03-22</t>
         </is>
       </c>
-      <c r="B230" t="n">
+      <c r="B285" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="231">
-      <c r="A231" t="inlineStr">
+    <row r="286">
+      <c r="A286" s="1" t="inlineStr">
         <is>
           <t>2020-03-21</t>
         </is>
       </c>
-      <c r="B231" t="n">
+      <c r="B286" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="232">
-      <c r="A232" t="inlineStr">
+    <row r="287">
+      <c r="A287" s="1" t="inlineStr">
         <is>
           <t>2020-03-20</t>
         </is>
       </c>
-      <c r="B232" t="n">
+      <c r="B287" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="233">
-      <c r="A233" t="inlineStr">
+    <row r="288">
+      <c r="A288" s="1" t="inlineStr">
         <is>
           <t>2020-03-19</t>
         </is>
       </c>
-      <c r="B233" t="n">
+      <c r="B288" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="234">
-      <c r="A234" t="inlineStr">
+    <row r="289">
+      <c r="A289" s="1" t="inlineStr">
         <is>
           <t>2020-03-18</t>
         </is>
       </c>
-      <c r="B234" t="n">
+      <c r="B289" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" t="inlineStr">
+    <row r="290">
+      <c r="A290" s="1" t="inlineStr">
         <is>
           <t>2020-03-17</t>
         </is>
       </c>
-      <c r="B235" t="n">
+      <c r="B290" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" t="inlineStr">
+    <row r="291">
+      <c r="A291" s="1" t="inlineStr">
         <is>
           <t>2020-03-16</t>
         </is>
       </c>
-      <c r="B236" t="n">
+      <c r="B291" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" t="inlineStr">
+    <row r="292">
+      <c r="A292" s="1" t="inlineStr">
         <is>
           <t>2020-03-15</t>
         </is>
       </c>
-      <c r="B237" t="n">
+      <c r="B292" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" t="inlineStr">
+    <row r="293">
+      <c r="A293" s="1" t="inlineStr">
         <is>
           <t>2020-03-14</t>
         </is>
       </c>
-      <c r="B238" t="n">
+      <c r="B293" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="239">
-      <c r="A239" t="inlineStr">
+    <row r="294">
+      <c r="A294" s="1" t="inlineStr">
         <is>
           <t>2020-03-13</t>
         </is>
       </c>
-      <c r="B239" t="n">
+      <c r="B294" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" t="inlineStr">
+    <row r="295">
+      <c r="A295" s="1" t="inlineStr">
         <is>
           <t>2020-03-12</t>
         </is>
       </c>
-      <c r="B240" t="n">
+      <c r="B295" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" t="inlineStr">
+    <row r="296">
+      <c r="A296" s="1" t="inlineStr">
         <is>
           <t>2020-03-11</t>
         </is>
       </c>
-      <c r="B241" t="n">
+      <c r="B296" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="242">
-      <c r="A242" t="inlineStr">
+    <row r="297">
+      <c r="A297" s="1" t="inlineStr">
         <is>
           <t>2020-03-10</t>
         </is>
       </c>
-      <c r="B242" t="n">
+      <c r="B297" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>